<commit_message>
Notas al 13 Oct 2022
</commit_message>
<xml_diff>
--- a/Notas UNSA 2022B.xlsx
+++ b/Notas UNSA 2022B.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlocorrales/Documents/UNSA/UNSAn/Notas UNSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A3CC14-4F7B-DF46-9B6A-CD32C7916B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BB3F27-897C-E944-A34F-43AB0478251F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="3" xr2:uid="{74783B82-D1FB-8943-B7B3-349A45D55DB2}"/>
+    <workbookView xWindow="1020" yWindow="1200" windowWidth="21520" windowHeight="16460" activeTab="3" xr2:uid="{74783B82-D1FB-8943-B7B3-349A45D55DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Teo A" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="281">
   <si>
     <t>CUI</t>
   </si>
@@ -879,6 +879,9 @@
   </si>
   <si>
     <t>Cmandos Moodle</t>
+  </si>
+  <si>
+    <t>Intervenciones</t>
   </si>
 </sst>
 </file>
@@ -1280,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A2D1FB-3F87-7043-9CAF-EA8686A2DBDA}">
-  <dimension ref="B2:D51"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D51"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,7 +1296,7 @@
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1303,8 +1306,11 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>101</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>104</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>106</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>108</v>
       </c>
@@ -1347,8 +1353,11 @@
       <c r="D6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>110</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>112</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>114</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>116</v>
       </c>
@@ -1392,7 +1401,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>118</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>120</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>124</v>
       </c>
@@ -1435,8 +1444,11 @@
       <c r="D14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>126</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>128</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>130</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>132</v>
       </c>
@@ -1480,7 +1492,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>134</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>136</v>
       </c>
@@ -1502,7 +1514,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>139</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>141</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>143</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>145</v>
       </c>
@@ -1546,7 +1558,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>147</v>
       </c>
@@ -1556,8 +1568,11 @@
       <c r="D25" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>150</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>152</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>154</v>
       </c>
@@ -1590,7 +1605,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>156</v>
       </c>
@@ -1601,7 +1616,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>158</v>
       </c>
@@ -1612,7 +1627,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>160</v>
       </c>
@@ -1622,8 +1637,11 @@
       <c r="D31" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>162</v>
       </c>
@@ -1634,7 +1652,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>164</v>
       </c>
@@ -1645,7 +1663,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>166</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>168</v>
       </c>
@@ -1667,7 +1685,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>170</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>172</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>174</v>
       </c>
@@ -1700,7 +1718,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>176</v>
       </c>
@@ -1711,7 +1729,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>178</v>
       </c>
@@ -1722,7 +1740,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>180</v>
       </c>
@@ -1733,7 +1751,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>182</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>184</v>
       </c>
@@ -1755,7 +1773,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>186</v>
       </c>
@@ -1766,7 +1784,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>188</v>
       </c>
@@ -1777,7 +1795,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>190</v>
       </c>
@@ -1788,7 +1806,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>192</v>
       </c>
@@ -1798,8 +1816,11 @@
       <c r="D47" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>194</v>
       </c>
@@ -1810,7 +1831,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>196</v>
       </c>
@@ -1820,8 +1841,11 @@
       <c r="D49" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>198</v>
       </c>
@@ -1832,7 +1856,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>200</v>
       </c>
@@ -1850,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2C9259-6AE3-4C4E-B6FE-6E5ACB3EDFF5}">
-  <dimension ref="B2:D51"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1863,7 +1887,7 @@
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1873,8 +1897,11 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>20143020</v>
       </c>
@@ -1885,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>20220596</v>
       </c>
@@ -1896,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>20223006</v>
       </c>
@@ -1907,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>20130597</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>20224226</v>
       </c>
@@ -1929,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>20182314</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>20223009</v>
       </c>
@@ -1951,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>20220566</v>
       </c>
@@ -1962,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>20222075</v>
       </c>
@@ -1973,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>20222073</v>
       </c>
@@ -1984,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>20223017</v>
       </c>
@@ -1995,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>20200593</v>
       </c>
@@ -2006,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>20210558</v>
       </c>
@@ -2017,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>20162887</v>
       </c>
@@ -2028,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>20200601</v>
       </c>
@@ -2039,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>20222060</v>
       </c>
@@ -2050,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>20223015</v>
       </c>
@@ -2061,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>20222059</v>
       </c>
@@ -2072,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>20200606</v>
       </c>
@@ -2083,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>20223019</v>
       </c>
@@ -2094,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>20220577</v>
       </c>
@@ -2105,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>20223011</v>
       </c>
@@ -2116,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>20171789</v>
       </c>
@@ -2127,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>20211779</v>
       </c>
@@ -2138,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>20220585</v>
       </c>
@@ -2149,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>20200585</v>
       </c>
@@ -2160,7 +2187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>20220594</v>
       </c>
@@ -2171,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>20222066</v>
       </c>
@@ -2182,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>20222079</v>
       </c>
@@ -2192,8 +2219,11 @@
       <c r="D31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>20220575</v>
       </c>
@@ -2204,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <v>20222078</v>
       </c>
@@ -2215,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <v>20164034</v>
       </c>
@@ -2226,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
         <v>20213040</v>
       </c>
@@ -2237,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
         <v>20222582</v>
       </c>
@@ -2248,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
         <v>20222058</v>
       </c>
@@ -2259,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>20222061</v>
       </c>
@@ -2270,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <v>20223007</v>
       </c>
@@ -2281,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <v>20220583</v>
       </c>
@@ -2292,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>20211788</v>
       </c>
@@ -2303,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
         <v>20220591</v>
       </c>
@@ -2314,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>20214260</v>
       </c>
@@ -2325,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>20123159</v>
       </c>
@@ -2336,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>20210555</v>
       </c>
@@ -2347,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
         <v>20211785</v>
       </c>
@@ -2357,8 +2387,11 @@
       <c r="D46" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>20213025</v>
       </c>
@@ -2369,7 +2402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
         <v>20193195</v>
       </c>
@@ -2420,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B550D9D-ADF0-0942-9E43-7987DF989747}">
-  <dimension ref="B2:D51"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D51"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2433,7 +2466,7 @@
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2443,8 +2476,11 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>20193546</v>
       </c>
@@ -2455,7 +2491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>20173377</v>
       </c>
@@ -2466,7 +2502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>20211778</v>
       </c>
@@ -2477,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>20222063</v>
       </c>
@@ -2488,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>20220572</v>
       </c>
@@ -2499,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>20200586</v>
       </c>
@@ -2510,7 +2546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>20220579</v>
       </c>
@@ -2521,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>20191426</v>
       </c>
@@ -2532,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>20213042</v>
       </c>
@@ -2543,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>20200603</v>
       </c>
@@ -2554,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>20210552</v>
       </c>
@@ -2565,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>20192188</v>
       </c>
@@ -2576,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>20173366</v>
       </c>
@@ -2587,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>20220569</v>
       </c>
@@ -2595,6 +2631,9 @@
         <v>65</v>
       </c>
       <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
     </row>
@@ -2993,7 +3032,7 @@
   <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3003,6 +3042,8 @@
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="20" x14ac:dyDescent="0.2">
@@ -3050,6 +3091,9 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
@@ -3067,6 +3111,9 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
@@ -3082,7 +3129,10 @@
         <v>214</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H5">
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="20" x14ac:dyDescent="0.2">
@@ -3101,6 +3151,9 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
@@ -3121,6 +3174,9 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -3141,6 +3197,9 @@
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="J8">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -3161,6 +3220,9 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="J9">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -3238,6 +3300,9 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
@@ -3275,6 +3340,9 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
@@ -3296,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B17" s="5">
         <v>15</v>
       </c>
@@ -3312,8 +3380,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B18" s="5">
         <v>16</v>
       </c>
@@ -3335,8 +3406,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -3356,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B20" s="5">
         <v>18</v>
       </c>
@@ -3376,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -3396,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B22" s="5">
         <v>20</v>
       </c>
@@ -3416,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -3432,8 +3506,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -3452,8 +3529,11 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="20" x14ac:dyDescent="0.2">
       <c r="B25" s="5">
         <v>23</v>
       </c>

</xml_diff>